<commit_message>
Tabular versions of excel files
</commit_message>
<xml_diff>
--- a/tabular/Africa/CosmoAf1cmiss.xlsx
+++ b/tabular/Africa/CosmoAf1cmiss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathr\Dropbox\GLUE\Whole clades\Completed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/NCBI-RABV-GLUE/tabular/Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928CD022-68A0-433A-9820-82E05B3BC9C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733D7971-D1DF-9B4D-92E4-55EB6F38C2D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -757,45 +757,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="Q5" sqref="A1:AH7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" style="1" customWidth="1"/>
-    <col min="9" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="16.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="18" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" customWidth="1"/>
-    <col min="24" max="24" width="23.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="26.42578125" customWidth="1"/>
-    <col min="26" max="26" width="22" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" customWidth="1"/>
-    <col min="28" max="28" width="14.140625" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" customWidth="1"/>
-    <col min="30" max="32" width="19.85546875" customWidth="1"/>
-    <col min="33" max="33" width="17" customWidth="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.5" style="1" customWidth="1"/>
+    <col min="9" max="13" width="9.1640625" style="1"/>
+    <col min="14" max="14" width="16.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="18" style="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="23.83203125" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.5" customWidth="1"/>
+    <col min="25" max="25" width="22" style="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" customWidth="1"/>
+    <col min="27" max="27" width="14.1640625" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" customWidth="1"/>
+    <col min="29" max="31" width="19.83203125" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,59 +840,59 @@
       <c r="P1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="R1" s="3" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="AD1" s="15" t="s">
+        <v>69</v>
+      </c>
       <c r="AE1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -942,57 +941,57 @@
       <c r="P2" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="R2" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="S2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="7">
+        <v>2001</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="7">
+        <v>2001</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" s="7">
-        <v>2001</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z2" s="7">
-        <v>2001</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="AE2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AF2" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG2" s="7" t="s">
+      <c r="AF2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AG2" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1041,60 +1040,60 @@
       <c r="P3" t="s">
         <v>48</v>
       </c>
+      <c r="Q3" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="R3" s="9" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="10">
+        <v>67</v>
+      </c>
+      <c r="U3" s="10">
         <v>1980</v>
       </c>
-      <c r="W3" s="9" t="s">
+      <c r="V3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="X3" s="10">
+      <c r="W3" s="10">
         <v>1980</v>
       </c>
-      <c r="Y3" s="9" t="s">
+      <c r="X3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Z3" s="11">
+      <c r="Y3" s="11">
         <v>1980</v>
       </c>
+      <c r="Z3" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="AA3" s="9" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD3" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="AE3" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AF3" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG3" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="AF3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1143,57 +1142,57 @@
       <c r="P4" t="s">
         <v>49</v>
       </c>
+      <c r="Q4" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="R4" s="12" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="V4" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="W4" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="X4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z4" s="12">
+        <v>67</v>
+      </c>
+      <c r="Y4" s="12">
         <v>2004</v>
       </c>
+      <c r="Z4" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA4" s="12" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="AB4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD4" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="AE4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AF4" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG4" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH4" s="8" t="s">
+      <c r="AF4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1242,57 +1241,57 @@
       <c r="P5" t="s">
         <v>50</v>
       </c>
+      <c r="Q5" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="R5" s="9" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="V5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="W5" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="X5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z5" s="9">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="9">
         <v>1998</v>
       </c>
+      <c r="Z5" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="AA5" s="9" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD5" s="9"/>
+        <v>67</v>
+      </c>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="AE5" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AF5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH5" s="8" t="s">
+      <c r="AF5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG5" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1341,57 +1340,57 @@
       <c r="P6" t="s">
         <v>51</v>
       </c>
+      <c r="Q6" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="R6" s="12" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="V6" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="W6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="W6" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="X6" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z6" s="12">
+        <v>67</v>
+      </c>
+      <c r="Y6" s="12">
         <v>1986</v>
       </c>
+      <c r="Z6" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="AA6" s="12" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="AB6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC6" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD6" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="AE6" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AF6" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG6" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH6" s="8" t="s">
+      <c r="AF6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG6" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1440,63 +1439,63 @@
       <c r="P7" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="Q7" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="R7" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="S7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" s="14">
+        <v>1995</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="X7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>1995</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB7" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="T7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="U7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="V7" s="14">
-        <v>1995</v>
-      </c>
-      <c r="W7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z7" s="14">
-        <v>1995</v>
-      </c>
-      <c r="AA7" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB7" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC7" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="17" t="s">
+        <v>71</v>
+      </c>
       <c r="AE7" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="AF7" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG7" s="14" t="s">
+      <c r="AF7" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AH7" s="2" t="s">
+      <c r="AG7" s="2" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S1:S1048576 U1:U1048576 W1:W1048576 Y1:Y1048576 AA1:AA1048576 AC1:AC1048576 AH1:AH1048576">
+  <conditionalFormatting sqref="R1:R1048576 T1:T1048576 V1:V1048576 X1:X1048576 Z1:Z1048576 AB1:AB1048576 AG1:AG1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="updated">
-      <formula>NOT(ISERROR(SEARCH("updated",S1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("updated",R1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="filled in">
-      <formula>NOT(ISERROR(SEARCH("filled in",S1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("filled in",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>